<commit_message>
just t some content entry left
</commit_message>
<xml_diff>
--- a/portfolio-coding.xlsx
+++ b/portfolio-coding.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="15560" yWindow="460" windowWidth="10000" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="3620" yWindow="460" windowWidth="19760" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Project</t>
   </si>
@@ -69,16 +69,59 @@
   </si>
   <si>
     <t>https://github.com/anrope/oldnews</t>
+  </si>
+  <si>
+    <t>Durham VOICE website</t>
+  </si>
+  <si>
+    <t>http://durhamvoice.org/</t>
+  </si>
+  <si>
+    <t>HTML/CSS, PHP, Wordpress CMS</t>
+  </si>
+  <si>
+    <t>SQL Library Project</t>
+  </si>
+  <si>
+    <t>Reese News Lab</t>
+  </si>
+  <si>
+    <t>Campaign Finance</t>
+  </si>
+  <si>
+    <t>Election Guide</t>
+  </si>
+  <si>
+    <t>Writing App</t>
+  </si>
+  <si>
+    <t>Driven Media</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,13 +144,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,73 +431,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <v>42339</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>